<commit_message>
Updated most of chapter 7. TODO: 7.6, and a section on constant arrays
</commit_message>
<xml_diff>
--- a/data/maingraphs-code-size-table.xlsx
+++ b/data/maingraphs-code-size-table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="33600" windowHeight="20540" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="main table" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="127">
   <si>
     <t>BENCHMARK x</t>
   </si>
@@ -6108,7 +6108,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+    <sheetView topLeftCell="A26" workbookViewId="0">
       <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
@@ -7843,7 +7843,7 @@
       </c>
       <c r="G49">
         <f>'mem usage'!C52</f>
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -7872,7 +7872,7 @@
       </c>
       <c r="G50" s="5">
         <f>'mem usage'!C52</f>
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -7901,7 +7901,7 @@
       </c>
       <c r="G51" s="5">
         <f>'mem usage'!D52</f>
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -7930,7 +7930,7 @@
       </c>
       <c r="G52" s="5">
         <f>'mem usage'!E52</f>
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -7959,7 +7959,7 @@
       </c>
       <c r="G53" s="5">
         <f>'mem usage'!F$52</f>
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -7988,7 +7988,7 @@
       </c>
       <c r="G54" s="5">
         <f>'mem usage'!F$52</f>
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -8017,7 +8017,7 @@
       </c>
       <c r="G55" s="5">
         <f>'mem usage'!F$52</f>
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -8046,7 +8046,7 @@
       </c>
       <c r="G56" s="5">
         <f>'mem usage'!F$52</f>
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -8075,7 +8075,7 @@
       </c>
       <c r="G57" s="5">
         <f>'mem usage'!F$52</f>
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -8093,8 +8093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K52"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8339,7 +8339,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="33" spans="5:11" ht="16">
+    <row r="33" spans="3:11" ht="16">
       <c r="G33" t="s">
         <v>119</v>
       </c>
@@ -8347,7 +8347,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="34" spans="5:11" ht="16">
+    <row r="34" spans="3:11" ht="16">
       <c r="E34">
         <v>2</v>
       </c>
@@ -8355,7 +8355,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="35" spans="5:11" ht="16">
+    <row r="35" spans="3:11" ht="16">
       <c r="E35">
         <v>2</v>
       </c>
@@ -8363,7 +8363,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="5:11" ht="16">
+    <row r="36" spans="3:11" ht="16">
       <c r="E36">
         <v>11</v>
       </c>
@@ -8371,7 +8371,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="37" spans="5:11" ht="16">
+    <row r="37" spans="3:11" ht="16">
       <c r="E37">
         <v>22</v>
       </c>
@@ -8379,7 +8379,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="38" spans="5:11" ht="16">
+    <row r="38" spans="3:11" ht="16">
       <c r="E38">
         <v>22</v>
       </c>
@@ -8387,7 +8387,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="39" spans="5:11" ht="16">
+    <row r="39" spans="3:11" ht="16">
       <c r="E39">
         <v>2</v>
       </c>
@@ -8395,7 +8395,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="40" spans="5:11" ht="16">
+    <row r="40" spans="3:11" ht="16">
       <c r="E40">
         <v>1</v>
       </c>
@@ -8403,17 +8403,17 @@
         <v>102</v>
       </c>
     </row>
-    <row r="41" spans="5:11" ht="16">
+    <row r="41" spans="3:11" ht="16">
       <c r="K41" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="42" spans="5:11" ht="16">
+    <row r="42" spans="3:11" ht="16">
       <c r="K42" s="8" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="43" spans="5:11" ht="16">
+    <row r="43" spans="3:11" ht="16">
       <c r="G43" t="s">
         <v>119</v>
       </c>
@@ -8421,7 +8421,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="44" spans="5:11" ht="16">
+    <row r="44" spans="3:11" ht="16">
       <c r="G44" t="s">
         <v>119</v>
       </c>
@@ -8429,7 +8429,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="45" spans="5:11" ht="16">
+    <row r="45" spans="3:11" ht="16">
       <c r="G45" t="s">
         <v>119</v>
       </c>
@@ -8437,7 +8437,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="46" spans="5:11" ht="16">
+    <row r="46" spans="3:11" ht="16">
       <c r="G46" t="s">
         <v>119</v>
       </c>
@@ -8445,17 +8445,17 @@
         <v>108</v>
       </c>
     </row>
-    <row r="47" spans="5:11" ht="16">
-      <c r="G47" t="s">
-        <v>119</v>
+    <row r="47" spans="3:11" ht="16">
+      <c r="C47">
+        <v>1</v>
       </c>
       <c r="K47" s="8" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="48" spans="5:11" ht="16">
-      <c r="G48" t="s">
-        <v>119</v>
+    <row r="48" spans="3:11" ht="16">
+      <c r="C48">
+        <v>1</v>
       </c>
       <c r="K48" s="8" t="s">
         <v>110</v>
@@ -8496,20 +8496,20 @@
     </row>
     <row r="52" spans="2:11">
       <c r="C52">
-        <f>SUM(C2:C16)</f>
-        <v>23</v>
+        <f>SUM(C2:C50)</f>
+        <v>25</v>
       </c>
       <c r="D52">
         <f>$C$52+SUM(D20)</f>
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E52">
         <f>$C$52+SUM(E25:E27)</f>
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F52">
         <f>C52+SUM(E34:E40)</f>
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added comment about constant array optimisation to vm size table
</commit_message>
<xml_diff>
--- a/data/maingraphs-code-size-table.xlsx
+++ b/data/maingraphs-code-size-table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="33600" windowHeight="20540" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="main table" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="127">
   <si>
     <t>BENCHMARK x</t>
   </si>
@@ -396,10 +396,13 @@
     <t>TAKEN FROM sumsum_codesize.txt</t>
   </si>
   <si>
-    <t>Before adding GETCONSTARRAY: 22363 bytes for full version</t>
-  </si>
-  <si>
     <t>UPDATED 20180305</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Before adding GETCONSTARRAY: 22363 bytes for full version, vs. 22533 after. </t>
+  </si>
+  <si>
+    <t>Increase because of Const shift: 170 bytes</t>
   </si>
 </sst>
 </file>
@@ -503,8 +506,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="215">
+  <cellStyleXfs count="219">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -733,7 +740,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="215">
+  <cellStyles count="219">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -841,6 +848,8 @@
     <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -948,6 +957,8 @@
     <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2950,7 +2961,7 @@
         <v>-13.599999999999994</v>
       </c>
       <c r="Q41" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="R41" s="10"/>
     </row>
@@ -3712,7 +3723,7 @@
         <v>49.9</v>
       </c>
       <c r="Q9" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="R9" s="10"/>
     </row>
@@ -6157,8 +6168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="G57" sqref="A48:G57"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6441,7 +6452,7 @@
         <v>11916</v>
       </c>
       <c r="T8" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U8" s="10"/>
     </row>
@@ -7784,6 +7795,9 @@
       <c r="C37" t="s">
         <v>67</v>
       </c>
+      <c r="G37" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="38" spans="1:16">
       <c r="A38" t="s">
@@ -7792,6 +7806,9 @@
       <c r="B38">
         <v>15847</v>
       </c>
+      <c r="G38" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="39" spans="1:16">
       <c r="A39" t="s">
@@ -7855,9 +7872,6 @@
       </c>
       <c r="B46">
         <v>22533</v>
-      </c>
-      <c r="O46" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="47" spans="1:16" s="3" customFormat="1">

</xml_diff>

<commit_message>
Added before/after optimisation to instr. exec. perc. in two tables
</commit_message>
<xml_diff>
--- a/data/maingraphs-code-size-table.xlsx
+++ b/data/maingraphs-code-size-table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="33600" windowHeight="20540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="main table" sheetId="1" r:id="rId1"/>
@@ -1290,8 +1290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:O48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44:N44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8156,7 +8156,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+    <sheetView topLeftCell="A36" workbookViewId="0">
       <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>

</xml_diff>